<commit_message>
initial lab setup, options modal, hud art
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8045A1D-047F-42AB-A7CE-092A0F0120EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322F202B-006F-4A88-9F3B-3DBF7A0B8465}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5085" yWindow="600" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Key</t>
   </si>
@@ -44,6 +44,78 @@
   </si>
   <si>
     <t>Cybrary Game</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>OPTIONS</t>
+  </si>
+  <si>
+    <t>sound</t>
+  </si>
+  <si>
+    <t>SOUND</t>
+  </si>
+  <si>
+    <t>speech</t>
+  </si>
+  <si>
+    <t>SPEECH</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>CLOSE</t>
+  </si>
+  <si>
+    <t>chain_of_custody</t>
+  </si>
+  <si>
+    <t>Chain of Custody</t>
+  </si>
+  <si>
+    <t>activity_log</t>
+  </si>
+  <si>
+    <t>Activity Log</t>
+  </si>
+  <si>
+    <t>help</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>disk_clone</t>
+  </si>
+  <si>
+    <t>Disk Clone</t>
+  </si>
+  <si>
+    <t>hard_disk_drive</t>
+  </si>
+  <si>
+    <t>Hard Disk Drive</t>
+  </si>
+  <si>
+    <t>usb_flash_drive</t>
+  </si>
+  <si>
+    <t>USB Flash Drive</t>
   </si>
 </sst>
 </file>
@@ -379,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,6 +501,102 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
"image drive cloning" stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322F202B-006F-4A88-9F3B-3DBF7A0B8465}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001B0082-1CAB-46CA-B501-EE6A13C24883}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5085" yWindow="600" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Key</t>
   </si>
@@ -103,9 +103,6 @@
     <t>disk_clone</t>
   </si>
   <si>
-    <t>Disk Clone</t>
-  </si>
-  <si>
     <t>hard_disk_drive</t>
   </si>
   <si>
@@ -116,6 +113,15 @@
   </si>
   <si>
     <t>USB Flash Drive</t>
+  </si>
+  <si>
+    <t>Disk to Image Clone</t>
+  </si>
+  <si>
+    <t>progress_cloning_drive</t>
+  </si>
+  <si>
+    <t>Cloning {0} to {1}</t>
   </si>
 </sst>
 </file>
@@ -451,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,23 +584,31 @@
         <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
         <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
         <v>30</v>
       </c>
-      <c r="B15" t="s">
-        <v>31</v>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
initial search modal, some initial plan for data inspection
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001B0082-1CAB-46CA-B501-EE6A13C24883}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1967227A-26D8-40A7-9301-208FD551BE84}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5085" yWindow="600" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Key</t>
   </si>
@@ -122,6 +122,18 @@
   </si>
   <si>
     <t>Cloning {0} to {1}</t>
+  </si>
+  <si>
+    <t>search_title</t>
+  </si>
+  <si>
+    <t>Search: {0}</t>
+  </si>
+  <si>
+    <t>search_button</t>
+  </si>
+  <si>
+    <t>SEARCH</t>
   </si>
 </sst>
 </file>
@@ -457,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,6 +623,22 @@
         <v>33</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
initial file inspector modal
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD3B2D8-EEEF-4DDE-98C9-B23CB0A754BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6595F127-DF7A-445D-87FE-D3DFA7A511A4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5490" yWindow="3360" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Key</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>search_result_title</t>
+  </si>
+  <si>
+    <t>file_inspect_title</t>
+  </si>
+  <si>
+    <t>File Inspect: {0}</t>
   </si>
 </sst>
 </file>
@@ -499,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,6 +715,14 @@
         <v>46</v>
       </c>
     </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
some more lab flow
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6595F127-DF7A-445D-87FE-D3DFA7A511A4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CF3689-4CF4-4AA9-A66C-4644E13B2ABD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5490" yWindow="3360" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Key</t>
   </si>
@@ -170,6 +170,18 @@
   </si>
   <si>
     <t>File Inspect: {0}</t>
+  </si>
+  <si>
+    <t>dataInvestigate_file_inspector</t>
+  </si>
+  <si>
+    <t>File Inspector</t>
+  </si>
+  <si>
+    <t>files</t>
+  </si>
+  <si>
+    <t>Files</t>
   </si>
 </sst>
 </file>
@@ -505,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,6 +735,22 @@
         <v>49</v>
       </c>
     </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
initial data for lab inspect, initial network log display
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CF3689-4CF4-4AA9-A66C-4644E13B2ABD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B37844-59BA-4CFA-99D8-2EDA9C476E02}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5490" yWindow="3360" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Key</t>
   </si>
@@ -182,6 +182,48 @@
   </si>
   <si>
     <t>Files</t>
+  </si>
+  <si>
+    <t>network_log_title</t>
+  </si>
+  <si>
+    <t>Network Log Viewer</t>
+  </si>
+  <si>
+    <t>network_active_connections</t>
+  </si>
+  <si>
+    <t>Active Connections</t>
+  </si>
+  <si>
+    <t>network_log_proto</t>
+  </si>
+  <si>
+    <t>Proto</t>
+  </si>
+  <si>
+    <t>network_log_local_addy</t>
+  </si>
+  <si>
+    <t>Local Address</t>
+  </si>
+  <si>
+    <t>network_log_foreign_addy</t>
+  </si>
+  <si>
+    <t>Foreign Address</t>
+  </si>
+  <si>
+    <t>network_log_state</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>network_log_pid</t>
+  </si>
+  <si>
+    <t>PID</t>
   </si>
 </sst>
 </file>
@@ -517,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,6 +793,62 @@
         <v>53</v>
       </c>
     </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
some cleanup, tune data, bug fixes, network log display logic
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B37844-59BA-4CFA-99D8-2EDA9C476E02}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28821D6-E160-4D22-9732-FFC53774058D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5490" yWindow="3360" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>Key</t>
   </si>
@@ -224,6 +224,42 @@
   </si>
   <si>
     <t>PID</t>
+  </si>
+  <si>
+    <t>network_log_state_listening</t>
+  </si>
+  <si>
+    <t>LISTENING</t>
+  </si>
+  <si>
+    <t>network_log_state_established</t>
+  </si>
+  <si>
+    <t>ESTABLISHED</t>
+  </si>
+  <si>
+    <t>network_log_state_close_wait</t>
+  </si>
+  <si>
+    <t>network_log_state_time_wait</t>
+  </si>
+  <si>
+    <t>CLOSE_WAIT</t>
+  </si>
+  <si>
+    <t>TIME_WAIT</t>
+  </si>
+  <si>
+    <t>dataInvestigate_network_log_inspector</t>
+  </si>
+  <si>
+    <t>Network Log</t>
+  </si>
+  <si>
+    <t>search_title_files</t>
+  </si>
+  <si>
+    <t>Search In Files: {0}</t>
   </si>
 </sst>
 </file>
@@ -559,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,130 +759,178 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>66</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
faux registry log modal, some tweaks
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28821D6-E160-4D22-9732-FFC53774058D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFC3D24-930F-4451-86FA-EAC5828BBA6D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5490" yWindow="3360" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>Key</t>
   </si>
@@ -260,6 +260,48 @@
   </si>
   <si>
     <t>Search In Files: {0}</t>
+  </si>
+  <si>
+    <t>registry_log_title</t>
+  </si>
+  <si>
+    <t>REGISTRY: Computer/HKEY_CURRENT_USER/Software/Macrohard/Doors/CurrentVersion/Run</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>registry_inspector</t>
+  </si>
+  <si>
+    <t>Registry Inspector</t>
+  </si>
+  <si>
+    <t>search_title_registry</t>
+  </si>
+  <si>
+    <t>Search In Registry: {0}</t>
+  </si>
+  <si>
+    <t>registry</t>
+  </si>
+  <si>
+    <t>Registry</t>
   </si>
 </sst>
 </file>
@@ -595,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,170 +809,226 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>73</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
initial malware check implement
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFC3D24-930F-4451-86FA-EAC5828BBA6D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEC0F41-C6F2-4682-88A5-8195A5E396E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5490" yWindow="3360" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>Key</t>
   </si>
@@ -302,6 +302,48 @@
   </si>
   <si>
     <t>Registry</t>
+  </si>
+  <si>
+    <t>malware_check_title</t>
+  </si>
+  <si>
+    <t>Malware Identifier</t>
+  </si>
+  <si>
+    <t>check</t>
+  </si>
+  <si>
+    <t>CHECK</t>
+  </si>
+  <si>
+    <t>malware_not_found</t>
+  </si>
+  <si>
+    <t>No malware found.</t>
+  </si>
+  <si>
+    <t>malware_trojan_title</t>
+  </si>
+  <si>
+    <t>malware_trojan_detail</t>
+  </si>
+  <si>
+    <t>malware_rat_title</t>
+  </si>
+  <si>
+    <t>malware_rat_detail</t>
+  </si>
+  <si>
+    <t>trojan</t>
+  </si>
+  <si>
+    <t>rat</t>
+  </si>
+  <si>
+    <t>trojan detail</t>
+  </si>
+  <si>
+    <t>rat detail</t>
   </si>
 </sst>
 </file>
@@ -637,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,298 +779,354 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="B41" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B43" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B44" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>86</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lab background, start and login art
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2827BAD1-35D1-483F-A7D0-3CA7FED8E188}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06374FAF-DD8C-433F-B808-C4673FB9B89E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5490" yWindow="3360" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5250" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
   <si>
     <t>Key</t>
   </si>
@@ -43,9 +43,6 @@
     <t>title</t>
   </si>
   <si>
-    <t>Cybrary Game</t>
-  </si>
-  <si>
     <t>options</t>
   </si>
   <si>
@@ -362,6 +359,45 @@
   </si>
   <si>
     <t>Checking Malware: {0}</t>
+  </si>
+  <si>
+    <t>Cybrary Quest</t>
+  </si>
+  <si>
+    <t>begin</t>
+  </si>
+  <si>
+    <t>BEGIN</t>
+  </si>
+  <si>
+    <t>enter_name_title</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Name:</t>
+  </si>
+  <si>
+    <t>enter_name_name</t>
+  </si>
+  <si>
+    <t>enter_name_initial</t>
+  </si>
+  <si>
+    <t>Initials:</t>
+  </si>
+  <si>
+    <t>confirm</t>
+  </si>
+  <si>
+    <t>CONFIRM</t>
+  </si>
+  <si>
+    <t>enter_name_placeholder</t>
+  </si>
+  <si>
+    <t>Enter Text…</t>
   </si>
 </sst>
 </file>
@@ -697,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,431 +780,479 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
+        <v>114</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>116</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>120</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>124</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B38" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B48" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="B49" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="B50" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="B51" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="B52" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="B53" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B54" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B55" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>97</v>
+      </c>
+      <c r="B56" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>99</v>
+      </c>
+      <c r="B57" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>100</v>
+      </c>
+      <c r="B58" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>101</v>
+      </c>
+      <c r="B59" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>102</v>
+      </c>
+      <c r="B60" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>111</v>
+      </c>
+      <c r="B61" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>109</v>
+      </c>
+      <c r="B62" t="s">
         <v>110</v>
-      </c>
-      <c r="B56" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
camera ui art stuff, initial volatile hud art, etc.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06374FAF-DD8C-433F-B808-C4673FB9B89E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE773AD6-A1C0-4E1B-AB66-152F58503B41}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13770" yWindow="2070" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
   <si>
     <t>Key</t>
   </si>
@@ -398,6 +398,96 @@
   </si>
   <si>
     <t>Enter Text…</t>
+  </si>
+  <si>
+    <t>preInvestigate_report_title</t>
+  </si>
+  <si>
+    <t>Preliminary Report</t>
+  </si>
+  <si>
+    <t>Volatile Data Acquisition</t>
+  </si>
+  <si>
+    <t>volatile_data_acquisition</t>
+  </si>
+  <si>
+    <t>System Time</t>
+  </si>
+  <si>
+    <t>Process Info</t>
+  </si>
+  <si>
+    <t>Network Info</t>
+  </si>
+  <si>
+    <t>User Info</t>
+  </si>
+  <si>
+    <t>Cache Info</t>
+  </si>
+  <si>
+    <t>time_days</t>
+  </si>
+  <si>
+    <t>Days:</t>
+  </si>
+  <si>
+    <t>time_hours</t>
+  </si>
+  <si>
+    <t>Hours:</t>
+  </si>
+  <si>
+    <t>time_minutes</t>
+  </si>
+  <si>
+    <t>Minutes:</t>
+  </si>
+  <si>
+    <t>time_seconds</t>
+  </si>
+  <si>
+    <t>Seconds:</t>
+  </si>
+  <si>
+    <t>time_milliseconds</t>
+  </si>
+  <si>
+    <t>Milliseconds:</t>
+  </si>
+  <si>
+    <t>time_ticks</t>
+  </si>
+  <si>
+    <t>Ticks:</t>
+  </si>
+  <si>
+    <t>time_shell_command</t>
+  </si>
+  <si>
+    <t>PS C:\\&gt; (get-date) - (gcim Win32_OperatingSystem).LastBootUpTime</t>
+  </si>
+  <si>
+    <t>volatile_data_SystemTime</t>
+  </si>
+  <si>
+    <t>volatile_data_ProcessInfo</t>
+  </si>
+  <si>
+    <t>volatile_data_NetworkInfo</t>
+  </si>
+  <si>
+    <t>volatile_data_UserInfo</t>
+  </si>
+  <si>
+    <t>volatile_data_CacheInfo</t>
+  </si>
+  <si>
+    <t>volatile_data_acquire_title</t>
+  </si>
+  <si>
+    <t>Acquiring: {0}</t>
   </si>
 </sst>
 </file>
@@ -733,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,6 +1345,126 @@
         <v>110</v>
       </c>
     </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>154</v>
+      </c>
+      <c r="B64" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>129</v>
+      </c>
+      <c r="B65" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>149</v>
+      </c>
+      <c r="B66" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>150</v>
+      </c>
+      <c r="B67" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>151</v>
+      </c>
+      <c r="B68" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>152</v>
+      </c>
+      <c r="B69" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>153</v>
+      </c>
+      <c r="B70" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>147</v>
+      </c>
+      <c r="B71" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>135</v>
+      </c>
+      <c r="B72" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>137</v>
+      </c>
+      <c r="B73" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>139</v>
+      </c>
+      <c r="B74" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>141</v>
+      </c>
+      <c r="B75" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>143</v>
+      </c>
+      <c r="B76" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>145</v>
+      </c>
+      <c r="B77" t="s">
+        <v>146</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
modals for volatile data acquisition
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE773AD6-A1C0-4E1B-AB66-152F58503B41}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578872A0-9E4D-4212-9F57-1496A3DD3302}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13770" yWindow="2070" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18015" yWindow="3360" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
   <si>
     <t>Key</t>
   </si>
@@ -488,6 +488,36 @@
   </si>
   <si>
     <t>Acquiring: {0}</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>cpu</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>memory</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
+  <si>
+    <t>network</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>cache_data_captured</t>
+  </si>
+  <si>
+    <t>Cache data copied: command history, clipboard, print spool files.</t>
   </si>
 </sst>
 </file>
@@ -823,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,194 +1305,234 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>93</v>
+        <v>156</v>
       </c>
       <c r="B54" t="s">
-        <v>94</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>108</v>
+        <v>158</v>
       </c>
       <c r="B55" t="s">
-        <v>107</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>97</v>
+        <v>160</v>
       </c>
       <c r="B56" t="s">
-        <v>98</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>99</v>
+        <v>162</v>
       </c>
       <c r="B57" t="s">
-        <v>103</v>
+        <v>163</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B58" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B59" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B60" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B61" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B62" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="B63" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>154</v>
+        <v>102</v>
       </c>
       <c r="B64" t="s">
-        <v>155</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="B65" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>149</v>
+        <v>109</v>
       </c>
       <c r="B66" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="B67" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B68" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="B69" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B70" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B71" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="B72" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="B73" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="B74" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B75" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B76" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>137</v>
+      </c>
+      <c r="B77" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>139</v>
+      </c>
+      <c r="B78" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>141</v>
+      </c>
+      <c r="B79" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>143</v>
+      </c>
+      <c r="B80" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>145</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B81" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>164</v>
+      </c>
+      <c r="B82" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
icons, ui stuff for item acquisition
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578872A0-9E4D-4212-9F57-1496A3DD3302}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95DBCC6-3F31-40FC-83FF-FBFC44E3761E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18015" yWindow="3360" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5595" yWindow="1920" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="193">
   <si>
     <t>Key</t>
   </si>
@@ -518,6 +518,87 @@
   </si>
   <si>
     <t>Cache data copied: command history, clipboard, print spool files.</t>
+  </si>
+  <si>
+    <t>acquisition_item_desktop</t>
+  </si>
+  <si>
+    <t>Desktop</t>
+  </si>
+  <si>
+    <t>acquisition_item_keyboard</t>
+  </si>
+  <si>
+    <t>Keyboard</t>
+  </si>
+  <si>
+    <t>acquisition_item_monitor</t>
+  </si>
+  <si>
+    <t>Monitor</t>
+  </si>
+  <si>
+    <t>acquisition_item_monitorCable</t>
+  </si>
+  <si>
+    <t>Monitor Cable</t>
+  </si>
+  <si>
+    <t>acquisition_item_mouse</t>
+  </si>
+  <si>
+    <t>Mouse</t>
+  </si>
+  <si>
+    <t>acquisition_item_networkCable</t>
+  </si>
+  <si>
+    <t>Network Cable</t>
+  </si>
+  <si>
+    <t>acquisition_item_powerCable</t>
+  </si>
+  <si>
+    <t>Power Cable</t>
+  </si>
+  <si>
+    <t>acquisition_item_usbStick</t>
+  </si>
+  <si>
+    <t>acquisition_item_deskFan</t>
+  </si>
+  <si>
+    <t>Desk Fan</t>
+  </si>
+  <si>
+    <t>acquisition_item_photo</t>
+  </si>
+  <si>
+    <t>Photo</t>
+  </si>
+  <si>
+    <t>acquisition_item_stapler</t>
+  </si>
+  <si>
+    <t>Stapler</t>
+  </si>
+  <si>
+    <t>acquisition_title</t>
+  </si>
+  <si>
+    <t>Acquisition</t>
+  </si>
+  <si>
+    <t>back</t>
+  </si>
+  <si>
+    <t>BACK</t>
+  </si>
+  <si>
+    <t>acquisition_items</t>
+  </si>
+  <si>
+    <t>Item(s):</t>
   </si>
 </sst>
 </file>
@@ -853,10 +934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,562 +1058,674 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>189</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>116</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>117</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B19" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="B35" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B39" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B42" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B44" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B45" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B46" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="B48" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B49" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B50" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B51" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B52" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B53" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>156</v>
+        <v>85</v>
       </c>
       <c r="B54" t="s">
-        <v>157</v>
+        <v>86</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B55" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B56" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B57" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>93</v>
+        <v>162</v>
       </c>
       <c r="B58" t="s">
-        <v>94</v>
+        <v>163</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="B59" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="B60" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B61" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B62" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B63" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B64" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B65" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B66" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="B67" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="B68" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="B69" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="B70" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B71" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B72" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B73" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B74" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B75" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="B76" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B77" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B78" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B79" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B80" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B81" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>145</v>
+      </c>
+      <c r="B82" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>164</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B83" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>166</v>
+      </c>
+      <c r="B84" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>176</v>
+      </c>
+      <c r="B89" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>178</v>
+      </c>
+      <c r="B90" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>180</v>
+      </c>
+      <c r="B91" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>181</v>
+      </c>
+      <c r="B92" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>183</v>
+      </c>
+      <c r="B93" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>185</v>
+      </c>
+      <c r="B94" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>187</v>
+      </c>
+      <c r="B95" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>191</v>
+      </c>
+      <c r="B96" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
activity log and chain of custody stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95DBCC6-3F31-40FC-83FF-FBFC44E3761E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA96A07-EECE-49DB-82DE-34C1A1C4FFB5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5595" yWindow="1920" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7095" yWindow="3405" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="215">
   <si>
     <t>Key</t>
   </si>
@@ -599,6 +599,72 @@
   </si>
   <si>
     <t>Item(s):</t>
+  </si>
+  <si>
+    <t>chain_custody_date</t>
+  </si>
+  <si>
+    <t>Date/Time Obtained: {0}</t>
+  </si>
+  <si>
+    <t>chain_custody_case_no</t>
+  </si>
+  <si>
+    <t>Case Number: {0}</t>
+  </si>
+  <si>
+    <t>chain_custody_released_by</t>
+  </si>
+  <si>
+    <t>Released By:</t>
+  </si>
+  <si>
+    <t>chain_custody_received_by</t>
+  </si>
+  <si>
+    <t>Received By:</t>
+  </si>
+  <si>
+    <t>chain_custody_purpose</t>
+  </si>
+  <si>
+    <t>Purpose of Custody:</t>
+  </si>
+  <si>
+    <t>chain_custody_header_item</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>chain_custody_header_desc</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>chain_custody_officer</t>
+  </si>
+  <si>
+    <t>Greg Furgenson (Evidence Technician)</t>
+  </si>
+  <si>
+    <t>chain_custody_purpose_1</t>
+  </si>
+  <si>
+    <t>chain_custody_purpose_2</t>
+  </si>
+  <si>
+    <t>chain_custody_purpose_3</t>
+  </si>
+  <si>
+    <t>Transport and secure all evidence to lab for investigation.</t>
+  </si>
+  <si>
+    <t>Return and secure storage devices.</t>
+  </si>
+  <si>
+    <t>Clone storage devices (hard disc drive inside desktop, USB flash drive) for investigation.</t>
   </si>
 </sst>
 </file>
@@ -934,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D96"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1728,6 +1794,94 @@
         <v>192</v>
       </c>
     </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>193</v>
+      </c>
+      <c r="B97" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>195</v>
+      </c>
+      <c r="B98" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>197</v>
+      </c>
+      <c r="B99" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>199</v>
+      </c>
+      <c r="B100" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>201</v>
+      </c>
+      <c r="B101" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>203</v>
+      </c>
+      <c r="B102" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>205</v>
+      </c>
+      <c r="B103" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>207</v>
+      </c>
+      <c r="B104" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>209</v>
+      </c>
+      <c r="B105" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>210</v>
+      </c>
+      <c r="B106" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>211</v>
+      </c>
+      <c r="B107" t="s">
+        <v>213</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
photo album and result
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA96A07-EECE-49DB-82DE-34C1A1C4FFB5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DA3CE2-948B-49AA-8CD0-FE23E6518E89}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7095" yWindow="3405" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="223">
   <si>
     <t>Key</t>
   </si>
@@ -665,6 +665,30 @@
   </si>
   <si>
     <t>Clone storage devices (hard disc drive inside desktop, USB flash drive) for investigation.</t>
+  </si>
+  <si>
+    <t>photo_album</t>
+  </si>
+  <si>
+    <t>Photo Album</t>
+  </si>
+  <si>
+    <t>photo_result</t>
+  </si>
+  <si>
+    <t>Photo Result</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>Percent:</t>
+  </si>
+  <si>
+    <t>Points:</t>
+  </si>
+  <si>
+    <t>points</t>
   </si>
 </sst>
 </file>
@@ -1000,10 +1024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D107"/>
+  <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1882,6 +1906,38 @@
         <v>213</v>
       </c>
     </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>215</v>
+      </c>
+      <c r="B108" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>217</v>
+      </c>
+      <c r="B109" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>222</v>
+      </c>
+      <c r="B110" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>219</v>
+      </c>
+      <c r="B111" t="s">
+        <v>220</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
added result modals for: pc verify, device acquisition, volatile data gather
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DA3CE2-948B-49AA-8CD0-FE23E6518E89}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156F3449-9FAB-42D0-8A6E-167CF3ABCC12}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7095" yWindow="3405" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6765" yWindow="2820" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="243">
   <si>
     <t>Key</t>
   </si>
@@ -689,6 +689,66 @@
   </si>
   <si>
     <t>points</t>
+  </si>
+  <si>
+    <t>pc_verify_result</t>
+  </si>
+  <si>
+    <t>PC Verify Result</t>
+  </si>
+  <si>
+    <t>pc_verify_check_network</t>
+  </si>
+  <si>
+    <t>Network Cable Unplugged</t>
+  </si>
+  <si>
+    <t>pc_verify_check_power</t>
+  </si>
+  <si>
+    <t>Check PC Power Status</t>
+  </si>
+  <si>
+    <t>pc_verify_capture_screen</t>
+  </si>
+  <si>
+    <t>Monitor Active Screen Pictured</t>
+  </si>
+  <si>
+    <t>volatile_gather_result</t>
+  </si>
+  <si>
+    <t>Volatile Data Acquisition Result</t>
+  </si>
+  <si>
+    <t>volatile_gather_result_order</t>
+  </si>
+  <si>
+    <t>volatile_gather_result_player_order</t>
+  </si>
+  <si>
+    <t>Recommended Order</t>
+  </si>
+  <si>
+    <t>Your Order</t>
+  </si>
+  <si>
+    <t>device_gather_result</t>
+  </si>
+  <si>
+    <t>Device Acquisition Result</t>
+  </si>
+  <si>
+    <t>Points/Penalty</t>
+  </si>
+  <si>
+    <t>points_penalty</t>
+  </si>
+  <si>
+    <t>Digital Investigation Suite</t>
+  </si>
+  <si>
+    <t>digital_investigation_suite</t>
   </si>
 </sst>
 </file>
@@ -1024,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D111"/>
+  <dimension ref="A1:D121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A111" sqref="A111"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A121" sqref="A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1932,10 +1992,90 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>240</v>
+      </c>
+      <c r="B111" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>219</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B112" t="s">
         <v>220</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>223</v>
+      </c>
+      <c r="B113" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>225</v>
+      </c>
+      <c r="B114" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>227</v>
+      </c>
+      <c r="B115" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>229</v>
+      </c>
+      <c r="B116" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>231</v>
+      </c>
+      <c r="B117" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>233</v>
+      </c>
+      <c r="B118" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>234</v>
+      </c>
+      <c r="B119" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>237</v>
+      </c>
+      <c r="B120" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>242</v>
+      </c>
+      <c r="B121" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
digital investigation modal and flow
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156F3449-9FAB-42D0-8A6E-167CF3ABCC12}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F1DB02-DF67-46AF-ADC6-FAAE2A36C380}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6765" yWindow="2820" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="255">
   <si>
     <t>Key</t>
   </si>
@@ -749,6 +749,42 @@
   </si>
   <si>
     <t>digital_investigation_suite</t>
+  </si>
+  <si>
+    <t>digital_investigation_req_message</t>
+  </si>
+  <si>
+    <t>You need to flag at least three items from the investigation to proceed.</t>
+  </si>
+  <si>
+    <t>digital_investigation_report</t>
+  </si>
+  <si>
+    <t>Digital Investigation Report</t>
+  </si>
+  <si>
+    <t>report</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>proceed</t>
+  </si>
+  <si>
+    <t>PROCEED</t>
+  </si>
+  <si>
+    <t>cancel</t>
+  </si>
+  <si>
+    <t>CANCEL</t>
+  </si>
+  <si>
+    <t>digital_investigation_report_confirm</t>
+  </si>
+  <si>
+    <t>Do you want to finish the report and proceed?</t>
   </si>
 </sst>
 </file>
@@ -1084,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:D127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A121" sqref="A121"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="B127" sqref="B127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,866 +1252,914 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>249</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>251</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>116</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>119</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>118</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B19" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B20" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>124</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="B37" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B38" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B41" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B43" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B44" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B45" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B46" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B47" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B48" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B49" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B50" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="B51" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B52" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B53" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B54" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>156</v>
+        <v>83</v>
       </c>
       <c r="B55" t="s">
-        <v>157</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>158</v>
+        <v>85</v>
       </c>
       <c r="B56" t="s">
-        <v>159</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B57" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B58" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>93</v>
+        <v>160</v>
       </c>
       <c r="B59" t="s">
-        <v>94</v>
+        <v>161</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>108</v>
+        <v>162</v>
       </c>
       <c r="B60" t="s">
-        <v>107</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B61" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B62" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B63" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B64" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B65" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B66" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B67" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="B68" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>154</v>
+        <v>109</v>
       </c>
       <c r="B69" t="s">
-        <v>155</v>
+        <v>110</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B70" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="B71" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="B72" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B73" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B74" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B75" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B76" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="B77" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="B78" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B79" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B80" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B81" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B82" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="B83" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="B84" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B85" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B86" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B87" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B88" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B89" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B90" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B91" t="s">
-        <v>29</v>
+        <v>177</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B92" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B93" t="s">
-        <v>184</v>
+        <v>29</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B94" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B95" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B96" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B97" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B98" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B99" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B100" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B101" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B102" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B103" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B104" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B105" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B106" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B107" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B108" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B109" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="B110" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>240</v>
+        <v>217</v>
       </c>
       <c r="B111" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B112" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>223</v>
+        <v>240</v>
       </c>
       <c r="B113" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B114" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B115" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B116" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B117" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B118" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B119" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B120" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
+        <v>234</v>
+      </c>
+      <c r="B121" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>237</v>
+      </c>
+      <c r="B122" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>242</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B123" t="s">
         <v>241</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>245</v>
+      </c>
+      <c r="B124" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>243</v>
+      </c>
+      <c r="B125" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>247</v>
+      </c>
+      <c r="B126" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>253</v>
+      </c>
+      <c r="B127" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dialogs and guides pre-investigate, parts of on-site
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F1DB02-DF67-46AF-ADC6-FAAE2A36C380}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE9B7D8-E72B-465F-85F4-3240C71741D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6765" yWindow="2820" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="301">
   <si>
     <t>Key</t>
   </si>
@@ -403,9 +403,6 @@
     <t>preInvestigate_report_title</t>
   </si>
   <si>
-    <t>Preliminary Report</t>
-  </si>
-  <si>
     <t>Volatile Data Acquisition</t>
   </si>
   <si>
@@ -785,6 +782,147 @@
   </si>
   <si>
     <t>Do you want to finish the report and proceed?</t>
+  </si>
+  <si>
+    <t>Mission Briefing</t>
+  </si>
+  <si>
+    <t>department_name</t>
+  </si>
+  <si>
+    <t>Cybrary Hero Agents</t>
+  </si>
+  <si>
+    <t>preInvestigate_report_detail</t>
+  </si>
+  <si>
+    <t>intro_dialog_1</t>
+  </si>
+  <si>
+    <t>Welcome to Cybrary Quest!</t>
+  </si>
+  <si>
+    <t>intro_dialog_2</t>
+  </si>
+  <si>
+    <t>intro_dialog_3</t>
+  </si>
+  <si>
+    <t>In this game you will be investigating a computer that has been compromised by a malicious software.</t>
+  </si>
+  <si>
+    <t>I will be guiding you throughout the process.</t>
+  </si>
+  <si>
+    <t>intro_dialog_4</t>
+  </si>
+  <si>
+    <t>proceed_desc</t>
+  </si>
+  <si>
+    <t>Press this button to proceed.</t>
+  </si>
+  <si>
+    <t>help_preinvestigate_1</t>
+  </si>
+  <si>
+    <t>Type in your name in the field, and press CONFIRM to continue.</t>
+  </si>
+  <si>
+    <t>First, type in your name. This will be used for display in reports and logs.</t>
+  </si>
+  <si>
+    <t>help_preinvestigate_2</t>
+  </si>
+  <si>
+    <t>The pre-investigation phase shows information regarding the clients, the situation, the legalities, the agents involved, and the equipment.</t>
+  </si>
+  <si>
+    <t>\nCase Number: {0}\nDepartment: {1}\nDate: {2}\n\nAgents: {3} (Investigator), {4} (Evidence Technician)\n\nEquipments: Camera, Volatile Data Extractor Software, Data Analysis Software, External HDD\n\nClient: Billy Bob International Burger\n\n&lt;size=16&gt;Scenario&lt;/size&gt;\n\nThe company's I.T. (Robert Bob) has determined that their database has been compromised, and suspects it possibly being stolen.\n\nLooking at the network log, there have been huge amounts of traffic coming from a particular employee: John Burg.\n\nAfter examining the employee's workstation, they have determined it to be infected. Not taking any chances, they decided to call us in to further investigate the situation.\n\n&lt;size=16&gt;Legal Info&lt;/size&gt;\n\nWe have a full warrant to seize all devices related to the investigation for forensic purposes. We also have permission to view any information contained in the seized devices.\n</t>
+  </si>
+  <si>
+    <t>activity_arrived_onsite</t>
+  </si>
+  <si>
+    <t>Arrived at the workstation.</t>
+  </si>
+  <si>
+    <t>activity_dialog_1</t>
+  </si>
+  <si>
+    <t>activity_dialog_2</t>
+  </si>
+  <si>
+    <t>activity_dialog_3</t>
+  </si>
+  <si>
+    <t>activity_dialog_4</t>
+  </si>
+  <si>
+    <t>Notice that a message above shows a log of your arrival.</t>
+  </si>
+  <si>
+    <t>These logs are needed for reviewing and evaluating the case, as well as providing consistency with the evidence.</t>
+  </si>
+  <si>
+    <t>You can review these activities at the bottom of the screen.</t>
+  </si>
+  <si>
+    <t>Photography of the workstation taken.</t>
+  </si>
+  <si>
+    <t>activity_photography_taken</t>
+  </si>
+  <si>
+    <t>take_photo_dialog_1</t>
+  </si>
+  <si>
+    <t>Now that you have arrived, first thing to do is to take pictures of the workstation.</t>
+  </si>
+  <si>
+    <t>take_photo_dialog_2</t>
+  </si>
+  <si>
+    <t>Make sure to take a good picture of where all the devices are positioned, along with its surrounding.</t>
+  </si>
+  <si>
+    <t>camera_click_desc</t>
+  </si>
+  <si>
+    <t>Press this button to take a picture.</t>
+  </si>
+  <si>
+    <t>camera_drag_desc</t>
+  </si>
+  <si>
+    <t>Drag the mouse around the screen to move the camera.</t>
+  </si>
+  <si>
+    <t>As an investigator, it is important for you to log your activities during the investigation.</t>
+  </si>
+  <si>
+    <t>activity_check_power_state</t>
+  </si>
+  <si>
+    <t>activity_power_state_on</t>
+  </si>
+  <si>
+    <t>verify_computer_power_1</t>
+  </si>
+  <si>
+    <t>The next thing to do is check if the computer’s power is on, and if so, to unplug the network cable to avoid further attack from the internet.</t>
+  </si>
+  <si>
+    <t>verify_computer_power_2</t>
+  </si>
+  <si>
+    <t>Simply move the mouse over items of interest, and click on it to take action.</t>
+  </si>
+  <si>
+    <t>Confirmed that the workstation computer's power is on.</t>
+  </si>
+  <si>
+    <t>Verify if the workstation computer's power is on.</t>
   </si>
 </sst>
 </file>
@@ -834,11 +972,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1120,10 +1261,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D127"/>
+  <dimension ref="A1:D150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="B127" sqref="B127"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,922 +1385,1106 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>188</v>
+      </c>
+      <c r="B13" t="s">
         <v>189</v>
-      </c>
-      <c r="B13" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>248</v>
+      </c>
+      <c r="B14" t="s">
         <v>249</v>
-      </c>
-      <c r="B14" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>250</v>
+      </c>
+      <c r="B15" t="s">
         <v>251</v>
-      </c>
-      <c r="B15" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>255</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B21" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B22" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B29" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="B38" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B42" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B43" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B45" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B47" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B48" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B49" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="B51" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B52" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B53" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B54" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B55" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B56" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>156</v>
+        <v>85</v>
       </c>
       <c r="B57" t="s">
-        <v>157</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B58" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B59" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B60" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>93</v>
+        <v>161</v>
       </c>
       <c r="B61" t="s">
-        <v>94</v>
+        <v>162</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="B62" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="B63" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B64" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B65" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B66" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B67" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B68" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B69" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="B70" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="B71" t="s">
-        <v>155</v>
+        <v>254</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>129</v>
+        <v>257</v>
       </c>
       <c r="B72" t="s">
-        <v>128</v>
+        <v>272</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B73" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="B74" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B75" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B76" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B77" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B78" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="B79" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B80" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B81" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B82" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B83" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B84" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
       <c r="B85" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="B86" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B87" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B88" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B89" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B90" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B91" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B92" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B93" t="s">
-        <v>29</v>
+        <v>176</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B94" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B95" t="s">
-        <v>184</v>
+        <v>29</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B96" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B97" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B98" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B99" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B100" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B101" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B102" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B103" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B104" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B105" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B106" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B107" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B108" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>208</v>
+      </c>
+      <c r="B109" t="s">
         <v>211</v>
-      </c>
-      <c r="B109" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B110" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B111" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>222</v>
+        <v>273</v>
       </c>
       <c r="B112" t="s">
-        <v>221</v>
+        <v>274</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>240</v>
+        <v>283</v>
       </c>
       <c r="B113" t="s">
-        <v>239</v>
+        <v>282</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>219</v>
+        <v>293</v>
       </c>
       <c r="B114" t="s">
-        <v>220</v>
+        <v>300</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>223</v>
+        <v>294</v>
       </c>
       <c r="B115" t="s">
-        <v>224</v>
+        <v>299</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="B116" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="B117" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B118" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="B119" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="B120" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="B121" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="B122" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="B123" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="B124" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="B125" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="B126" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
+        <v>233</v>
+      </c>
+      <c r="B127" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>236</v>
+      </c>
+      <c r="B128" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>241</v>
+      </c>
+      <c r="B129" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>244</v>
+      </c>
+      <c r="B130" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>242</v>
+      </c>
+      <c r="B131" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>246</v>
+      </c>
+      <c r="B132" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>252</v>
+      </c>
+      <c r="B133" t="s">
         <v>253</v>
       </c>
-      <c r="B127" t="s">
-        <v>254</v>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>265</v>
+      </c>
+      <c r="B134" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>288</v>
+      </c>
+      <c r="B135" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>290</v>
+      </c>
+      <c r="B136" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>267</v>
+      </c>
+      <c r="B137" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>270</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>258</v>
+      </c>
+      <c r="B139" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>260</v>
+      </c>
+      <c r="B140" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>261</v>
+      </c>
+      <c r="B141" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>264</v>
+      </c>
+      <c r="B142" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>275</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>276</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>277</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>278</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>284</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>286</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>295</v>
+      </c>
+      <c r="B149" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>297</v>
+      </c>
+      <c r="B150" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more on-site help/guide crap
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE9B7D8-E72B-465F-85F4-3240C71741D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337EDBCF-D7DC-422C-A8F4-70B48EFD494B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6765" yWindow="2820" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8115" yWindow="3450" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="322">
   <si>
     <t>Key</t>
   </si>
@@ -859,9 +859,6 @@
     <t>activity_dialog_4</t>
   </si>
   <si>
-    <t>Notice that a message above shows a log of your arrival.</t>
-  </si>
-  <si>
     <t>These logs are needed for reviewing and evaluating the case, as well as providing consistency with the evidence.</t>
   </si>
   <si>
@@ -916,13 +913,79 @@
     <t>verify_computer_power_2</t>
   </si>
   <si>
-    <t>Simply move the mouse over items of interest, and click on it to take action.</t>
-  </si>
-  <si>
-    <t>Confirmed that the workstation computer's power is on.</t>
-  </si>
-  <si>
     <t>Verify if the workstation computer's power is on.</t>
+  </si>
+  <si>
+    <t>volatile_acquisition_dialog_1</t>
+  </si>
+  <si>
+    <t>Since the computer's power is on, we will have to acquire the volatile data.</t>
+  </si>
+  <si>
+    <t>volatile_acquisition_dialog_2</t>
+  </si>
+  <si>
+    <t>volatile_acquisition_dialog_3</t>
+  </si>
+  <si>
+    <t>volatile_acquisition_dialog_4</t>
+  </si>
+  <si>
+    <t>These are data that are lost once the computer is shut down.</t>
+  </si>
+  <si>
+    <t>The following are the kind of volatile data you will want to gather: system time, RAM, process information, network log, logged-on users' information, and cached data (command history, clipboard, print spool files).</t>
+  </si>
+  <si>
+    <t>help_volatile_gather</t>
+  </si>
+  <si>
+    <t>Click on any of the software's icon to execute it. Once you have gathered all the data, you can proceed.</t>
+  </si>
+  <si>
+    <t>Volatile data acquisition completed. Stored on HDD External drive (serial: 4487365-qq-78)</t>
+  </si>
+  <si>
+    <t>Confirmed that the workstation computer's power is on. Volatile data acquisition required.</t>
+  </si>
+  <si>
+    <t>Please ensure you gather the data in the order of most to least volatile. The most volatile data are the ones that change consistently as time goes on, and the least being the ones that rarely change.</t>
+  </si>
+  <si>
+    <t>activity_volatile_gather_complete</t>
+  </si>
+  <si>
+    <t>device_gather_dialog_1</t>
+  </si>
+  <si>
+    <t>Notice the message above indicating of your arrival.</t>
+  </si>
+  <si>
+    <t>Now that we have gathered the volatile data, the computer can now be shut down.</t>
+  </si>
+  <si>
+    <t>device_gather_dialog_2</t>
+  </si>
+  <si>
+    <t>All devices related to the investigation can now be packed up, and transfer to the lab for further inspection.</t>
+  </si>
+  <si>
+    <t>device_gather_dialog_3</t>
+  </si>
+  <si>
+    <t>Make sure to only take the devices that are used with the computer.</t>
+  </si>
+  <si>
+    <t>To interact with an item: move the mouse over an item of interest, and click on it.</t>
+  </si>
+  <si>
+    <t>activity_device_gather_complete</t>
+  </si>
+  <si>
+    <t>Packed up devices on workstation. Returning to the lab for further investigation.</t>
+  </si>
+  <si>
+    <t>chain_of_custody_dialog_1</t>
   </si>
 </sst>
 </file>
@@ -1261,10 +1324,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D150"/>
+  <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B115" sqref="B115"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="B161" sqref="B161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2185,306 +2248,391 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B113" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B114" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B115" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>214</v>
+        <v>310</v>
       </c>
       <c r="B116" t="s">
-        <v>215</v>
+        <v>307</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>216</v>
+        <v>319</v>
       </c>
       <c r="B117" t="s">
-        <v>217</v>
+        <v>320</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B118" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="B119" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B120" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>222</v>
+        <v>239</v>
       </c>
       <c r="B121" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B122" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B123" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B124" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B125" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B126" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B127" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B128" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B129" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B130" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B131" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B132" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="B133" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="B134" t="s">
-        <v>266</v>
+        <v>247</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
       <c r="B135" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>290</v>
+        <v>265</v>
       </c>
       <c r="B136" t="s">
-        <v>291</v>
+        <v>266</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="B137" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>270</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>271</v>
+        <v>289</v>
+      </c>
+      <c r="B138" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="B139" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>260</v>
-      </c>
-      <c r="B140" t="s">
-        <v>262</v>
+        <v>270</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>261</v>
-      </c>
-      <c r="B141" t="s">
-        <v>263</v>
+        <v>305</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="B142" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>275</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>279</v>
+        <v>260</v>
+      </c>
+      <c r="B143" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>276</v>
-      </c>
-      <c r="B144" s="3" t="s">
-        <v>292</v>
+        <v>261</v>
+      </c>
+      <c r="B144" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>277</v>
-      </c>
-      <c r="B145" s="3" t="s">
-        <v>280</v>
+        <v>264</v>
+      </c>
+      <c r="B145" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>281</v>
+        <v>312</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>295</v>
-      </c>
-      <c r="B149" t="s">
-        <v>296</v>
+        <v>278</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>297</v>
-      </c>
-      <c r="B150" t="s">
+        <v>283</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>285</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>294</v>
+      </c>
+      <c r="B152" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>296</v>
+      </c>
+      <c r="B153" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>298</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>300</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>301</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>302</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>311</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>314</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>316</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lab guide/info/final flow, end stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337EDBCF-D7DC-422C-A8F4-70B48EFD494B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05DDA6A-6EED-4160-84DA-585F8187BE9D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8115" yWindow="3450" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1215" yWindow="3615" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="395">
   <si>
     <t>Key</t>
   </si>
@@ -331,18 +331,6 @@
     <t>malware_rat_detail</t>
   </si>
   <si>
-    <t>trojan</t>
-  </si>
-  <si>
-    <t>rat</t>
-  </si>
-  <si>
-    <t>trojan detail</t>
-  </si>
-  <si>
-    <t>rat detail</t>
-  </si>
-  <si>
     <t>Malware Found</t>
   </si>
   <si>
@@ -838,9 +826,6 @@
     <t>The pre-investigation phase shows information regarding the clients, the situation, the legalities, the agents involved, and the equipment.</t>
   </si>
   <si>
-    <t>\nCase Number: {0}\nDepartment: {1}\nDate: {2}\n\nAgents: {3} (Investigator), {4} (Evidence Technician)\n\nEquipments: Camera, Volatile Data Extractor Software, Data Analysis Software, External HDD\n\nClient: Billy Bob International Burger\n\n&lt;size=16&gt;Scenario&lt;/size&gt;\n\nThe company's I.T. (Robert Bob) has determined that their database has been compromised, and suspects it possibly being stolen.\n\nLooking at the network log, there have been huge amounts of traffic coming from a particular employee: John Burg.\n\nAfter examining the employee's workstation, they have determined it to be infected. Not taking any chances, they decided to call us in to further investigate the situation.\n\n&lt;size=16&gt;Legal Info&lt;/size&gt;\n\nWe have a full warrant to seize all devices related to the investigation for forensic purposes. We also have permission to view any information contained in the seized devices.\n</t>
-  </si>
-  <si>
     <t>activity_arrived_onsite</t>
   </si>
   <si>
@@ -961,9 +946,6 @@
     <t>Notice the message above indicating of your arrival.</t>
   </si>
   <si>
-    <t>Now that we have gathered the volatile data, the computer can now be shut down.</t>
-  </si>
-  <si>
     <t>device_gather_dialog_2</t>
   </si>
   <si>
@@ -986,6 +968,243 @@
   </si>
   <si>
     <t>chain_of_custody_dialog_1</t>
+  </si>
+  <si>
+    <t>Now that we have gathered the volatile data, the computer can be shut down.</t>
+  </si>
+  <si>
+    <t>Before transferring the items, a Chain of Custody document must be made.</t>
+  </si>
+  <si>
+    <t>Think of the Chain of Custody document as a map of who/what/when/where/why of all the items from start to finish.</t>
+  </si>
+  <si>
+    <t>The labelling of items can depend on the department, and typically has a sequential number. In this case it is: the investigator’s initials, date, sequence number, sub-sequence number if attached from another item.</t>
+  </si>
+  <si>
+    <t>The Chain of Custody helps ensure that all the evidences gathered are genuine, and can be used at the court of law.</t>
+  </si>
+  <si>
+    <t>chain_of_custody_dialog_2</t>
+  </si>
+  <si>
+    <t>chain_of_custody_dialog_3</t>
+  </si>
+  <si>
+    <t>chain_of_custody_dialog_4</t>
+  </si>
+  <si>
+    <t>chain_of_custody_dialog_end</t>
+  </si>
+  <si>
+    <t>You can review the current Chain of Custody document at the bottom. Otherwise, we are ready to move on to the lab.</t>
+  </si>
+  <si>
+    <t>chain_custody_department</t>
+  </si>
+  <si>
+    <t>Department: {0}</t>
+  </si>
+  <si>
+    <t>activity_arrived_lab</t>
+  </si>
+  <si>
+    <t>Arrived at the lab.</t>
+  </si>
+  <si>
+    <t>lab_intro_dialog_1</t>
+  </si>
+  <si>
+    <t>Now that you are back in the lab, the first thing to do is grab the devices we need to investigate.</t>
+  </si>
+  <si>
+    <t>When doing digital forensics, it is best to avoid using the evidences directly when investigating. In this case, we will simply clone the disk drives.</t>
+  </si>
+  <si>
+    <t>lab_intro_clone_dialog_1</t>
+  </si>
+  <si>
+    <t>There are various ways to clone a disk drive, and that depends on the investigation. For our purpose, we just need to create an image file.</t>
+  </si>
+  <si>
+    <t>An image file contains a replication of all the data written on the disk. Certain software can navigate through that data as if it were an actual disk drive.</t>
+  </si>
+  <si>
+    <t>lab_intro_clone_dialog_2</t>
+  </si>
+  <si>
+    <t>lab_intro_clone_dialog_3</t>
+  </si>
+  <si>
+    <t>Simply click on the arrow icon to copy the drive to an image file.</t>
+  </si>
+  <si>
+    <t>help_hdd_clone</t>
+  </si>
+  <si>
+    <t>activity_clone_drives</t>
+  </si>
+  <si>
+    <t>Cloning disk drives to image files.</t>
+  </si>
+  <si>
+    <t>activity_investigate_data</t>
+  </si>
+  <si>
+    <t>Investigating image files.</t>
+  </si>
+  <si>
+    <t>activity_investigate_data_complete</t>
+  </si>
+  <si>
+    <t>Finished investigating image files. Found evidence of malware infection.</t>
+  </si>
+  <si>
+    <t>\nCase Number: {0}\nDepartment: {1}\nDate: {2}\n\nAgents: {3} (Investigator), {4} (Evidence Technician)\n\nEquipments: Camera, Volatile Data Extractor Software, Data Analysis Software, External HDD\n\nClient: Billy Bob International Burger\n\n&lt;size=16&gt;Scenario&lt;/size&gt;\n\nThe company's I.T. (Robert Bob) has determined that their database has been compromised, and suspects it possibly being stolen.\n\nLooking at the network log, there have been huge amounts of traffic coming from a particular employee: John Burg.\n\nAfter examining the employee's workstation, they noticed from the network log that a foreign IP address: 240.1.2.3 has established a connection to their server. Not taking any chances, they decided to call us in to further investigate the situation.\n\n&lt;size=16&gt;Legal Info&lt;/size&gt;\n\nWe have a full warrant to seize all devices related to the investigation for forensic purposes. We also have permission to view any information contained in the seized devices.\n</t>
+  </si>
+  <si>
+    <t>lab_investigate_dialog_1</t>
+  </si>
+  <si>
+    <t>With the image files, we can now begin our investigation.</t>
+  </si>
+  <si>
+    <t>lab_investigate_dialog_2</t>
+  </si>
+  <si>
+    <t>When it comes to analyzing data, the good approach is to look for patterns. Perhaps some initial information to use for search.</t>
+  </si>
+  <si>
+    <t>In this case, we can use our initial information from the briefing - the IP address: 240.1.2.3.</t>
+  </si>
+  <si>
+    <t>lab_investigate_dialog_3</t>
+  </si>
+  <si>
+    <t>help_data_investigate_1</t>
+  </si>
+  <si>
+    <t>In order to simplify the investigation, our software will only allow searches on flagged items. Our initial clue is the IP address: 240.1.2.3, this can be flagged from Network Log.</t>
+  </si>
+  <si>
+    <t>help_data_investigate_2</t>
+  </si>
+  <si>
+    <t>help_data_investigate_3</t>
+  </si>
+  <si>
+    <t>help_data_investigate_4</t>
+  </si>
+  <si>
+    <t>When you feel you are ready to finish the investigation, you can click on Report and proceed from there.</t>
+  </si>
+  <si>
+    <t>Once you have the IP address flagged in Network Log, you can then search for it in File Inspector. Other flagged items can show up in the other software.</t>
+  </si>
+  <si>
+    <t>Don't forget to identify any malware from the flagged files in Malware Identifier.</t>
+  </si>
+  <si>
+    <t>Trojan - Dropper</t>
+  </si>
+  <si>
+    <t>This type of Trojan malware will extract and execute another type of malware to the computer. They are typically under a guise of a legitimate software, and when run, will execute its malicious command invisible to the user.</t>
+  </si>
+  <si>
+    <t>RAT</t>
+  </si>
+  <si>
+    <t>A Remote Access Trojan (RAT) is a type of malware that allows hackers remote access to the user’s computer. This malware is typically injected to a user’s computer by some means, such as a Trojan, or through a website.</t>
+  </si>
+  <si>
+    <t>flagged_IP_desc</t>
+  </si>
+  <si>
+    <t>flagged_IP_in_file_desc</t>
+  </si>
+  <si>
+    <t>flagged_xkdc_exe_desc</t>
+  </si>
+  <si>
+    <t>flagged_xkdc_exe_in_file_desc</t>
+  </si>
+  <si>
+    <t>flagged_xkdc_exe_in_registry_desc</t>
+  </si>
+  <si>
+    <t>flagged_winampp_exe_desc</t>
+  </si>
+  <si>
+    <t>flagged_winampp_exe_in_file_desc</t>
+  </si>
+  <si>
+    <t>flagged_music_player_zip_desc</t>
+  </si>
+  <si>
+    <t>The IP address that is accessing the company's server through the infected workstation.</t>
+  </si>
+  <si>
+    <t>This file appears when searching for the IP address: 240.1.2.3.</t>
+  </si>
+  <si>
+    <t>Found inside winampp.exe, this indicates that the file is responsible for generating the RAT infection.</t>
+  </si>
+  <si>
+    <t>This executable appears to be an audio player of sort, and a trojan for installing xkdc.exe.</t>
+  </si>
+  <si>
+    <t>Found inside a compressed package: music_player.zip.</t>
+  </si>
+  <si>
+    <t>Found inside xkdc.exe, this indicates the file to be the source of access to the company's server.</t>
+  </si>
+  <si>
+    <t>Found when searching for \"winampp\", this is the compressed package that contains winampp.exe.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Found in the registry key: \"Computer/HKEY_CURRENT_USER/Software/Macrohard/Doors/CurrentVersion/Run\". This allows for the RAT infection to run at the OS start-up. </t>
+  </si>
+  <si>
+    <t>lab_investigate_post_dialog_1</t>
+  </si>
+  <si>
+    <t>Now that the malware is found along with its source, we can now report back to the client, and take the necessary steps to prevent future attacks from happening.</t>
+  </si>
+  <si>
+    <t>end_dialog_1</t>
+  </si>
+  <si>
+    <t>This concludes Cybrary Quest. You can review the report from here, and when you are done, click on the COMPLETE button.</t>
+  </si>
+  <si>
+    <t>end_dialog_2</t>
+  </si>
+  <si>
+    <t>Thank you for playing!</t>
+  </si>
+  <si>
+    <t>points_total</t>
+  </si>
+  <si>
+    <t>Total Points:</t>
+  </si>
+  <si>
+    <t>points_total_format</t>
+  </si>
+  <si>
+    <t>{0} out of {1}</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>COMPLETE</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
+  <si>
+    <t>Review</t>
   </si>
 </sst>
 </file>
@@ -1324,10 +1543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D161"/>
+  <dimension ref="A1:D197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="B161" sqref="B161"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1371,15 +1590,15 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1440,431 +1659,431 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B13" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B14" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B15" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>255</v>
+        <v>391</v>
       </c>
       <c r="B16" t="s">
-        <v>256</v>
+        <v>392</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>251</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>252</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>119</v>
+        <v>393</v>
       </c>
       <c r="B21" t="s">
-        <v>118</v>
+        <v>394</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B22" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B23" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>116</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>120</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B42" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B43" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B44" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B45" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B46" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B49" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B50" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B51" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B52" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B53" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="B54" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B55" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B56" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B57" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>155</v>
+        <v>83</v>
       </c>
       <c r="B58" t="s">
-        <v>156</v>
+        <v>84</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
       <c r="B59" t="s">
-        <v>158</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B60" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B61" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>93</v>
+        <v>155</v>
       </c>
       <c r="B62" t="s">
-        <v>94</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
       <c r="B63" t="s">
-        <v>107</v>
+        <v>158</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B64" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B65" t="s">
         <v>103</v>
@@ -1872,503 +2091,503 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B66" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B67" t="s">
-        <v>104</v>
+        <v>361</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B68" t="s">
-        <v>106</v>
+        <v>362</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B69" t="s">
-        <v>112</v>
+        <v>363</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B70" t="s">
-        <v>110</v>
+        <v>364</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="B71" t="s">
-        <v>254</v>
+        <v>108</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>257</v>
+        <v>105</v>
       </c>
       <c r="B72" t="s">
-        <v>272</v>
+        <v>106</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>153</v>
+        <v>122</v>
       </c>
       <c r="B73" t="s">
-        <v>154</v>
+        <v>250</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>128</v>
+        <v>253</v>
       </c>
       <c r="B74" t="s">
-        <v>127</v>
+        <v>346</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B75" t="s">
-        <v>129</v>
+        <v>150</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="B76" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B77" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B78" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B79" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B80" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="B81" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B82" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B83" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B84" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B85" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B86" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="B87" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="B88" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B89" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B90" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B91" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B92" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B93" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B94" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B95" t="s">
-        <v>29</v>
+        <v>172</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B96" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B97" t="s">
-        <v>183</v>
+        <v>29</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B98" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B99" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="B100" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="B101" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B102" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B103" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B104" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>200</v>
+        <v>326</v>
       </c>
       <c r="B105" t="s">
-        <v>201</v>
+        <v>327</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="B106" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="B107" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B108" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B109" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B110" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B111" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>273</v>
+        <v>204</v>
       </c>
       <c r="B112" t="s">
-        <v>274</v>
+        <v>207</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>282</v>
+        <v>205</v>
       </c>
       <c r="B113" t="s">
-        <v>281</v>
+        <v>209</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>292</v>
+        <v>206</v>
       </c>
       <c r="B114" t="s">
-        <v>297</v>
+        <v>208</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>293</v>
+        <v>268</v>
       </c>
       <c r="B115" t="s">
-        <v>308</v>
+        <v>269</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>310</v>
+        <v>277</v>
       </c>
       <c r="B116" t="s">
-        <v>307</v>
+        <v>276</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>319</v>
+        <v>287</v>
       </c>
       <c r="B117" t="s">
-        <v>320</v>
+        <v>292</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>214</v>
+        <v>288</v>
       </c>
       <c r="B118" t="s">
-        <v>215</v>
+        <v>303</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>216</v>
+        <v>305</v>
       </c>
       <c r="B119" t="s">
-        <v>217</v>
+        <v>302</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>221</v>
+        <v>313</v>
       </c>
       <c r="B120" t="s">
-        <v>220</v>
+        <v>314</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>239</v>
+        <v>328</v>
       </c>
       <c r="B121" t="s">
-        <v>238</v>
+        <v>329</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>218</v>
+        <v>340</v>
       </c>
       <c r="B122" t="s">
-        <v>219</v>
+        <v>341</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>222</v>
+        <v>342</v>
       </c>
       <c r="B123" t="s">
-        <v>223</v>
+        <v>343</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>224</v>
+        <v>344</v>
       </c>
       <c r="B124" t="s">
-        <v>225</v>
+        <v>345</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="B125" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="B126" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="B127" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B128" t="s">
         <v>234</v>
@@ -2376,263 +2595,554 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="B129" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>236</v>
+        <v>387</v>
       </c>
       <c r="B130" t="s">
-        <v>237</v>
+        <v>388</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>241</v>
+        <v>389</v>
       </c>
       <c r="B131" t="s">
-        <v>240</v>
+        <v>390</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="B132" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>242</v>
+        <v>220</v>
       </c>
       <c r="B133" t="s">
-        <v>243</v>
+        <v>221</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="B134" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>252</v>
+        <v>224</v>
       </c>
       <c r="B135" t="s">
-        <v>253</v>
+        <v>225</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>265</v>
+        <v>226</v>
       </c>
       <c r="B136" t="s">
-        <v>266</v>
+        <v>227</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>287</v>
+        <v>228</v>
       </c>
       <c r="B137" t="s">
-        <v>288</v>
+        <v>230</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>289</v>
+        <v>229</v>
       </c>
       <c r="B138" t="s">
-        <v>290</v>
+        <v>231</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="B139" t="s">
-        <v>268</v>
+        <v>233</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>270</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>271</v>
+        <v>237</v>
+      </c>
+      <c r="B140" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>305</v>
-      </c>
-      <c r="B141" s="3" t="s">
-        <v>306</v>
+        <v>240</v>
+      </c>
+      <c r="B141" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="B142" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="B143" t="s">
-        <v>262</v>
+        <v>243</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="B144" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B145" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>275</v>
-      </c>
-      <c r="B146" s="3" t="s">
-        <v>312</v>
+        <v>282</v>
+      </c>
+      <c r="B146" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>276</v>
-      </c>
-      <c r="B147" s="3" t="s">
-        <v>291</v>
+        <v>284</v>
+      </c>
+      <c r="B147" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>277</v>
-      </c>
-      <c r="B148" s="3" t="s">
-        <v>279</v>
+        <v>263</v>
+      </c>
+      <c r="B148" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>283</v>
+        <v>300</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>284</v>
+        <v>301</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>285</v>
-      </c>
-      <c r="B151" s="3" t="s">
-        <v>286</v>
+        <v>339</v>
+      </c>
+      <c r="B151" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>294</v>
+        <v>353</v>
       </c>
       <c r="B152" t="s">
-        <v>295</v>
+        <v>354</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>296</v>
-      </c>
-      <c r="B153" t="s">
-        <v>318</v>
+        <v>355</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>298</v>
+        <v>356</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>299</v>
+        <v>360</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>300</v>
-      </c>
-      <c r="B155" s="3" t="s">
-        <v>303</v>
+        <v>357</v>
+      </c>
+      <c r="B155" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>301</v>
-      </c>
-      <c r="B156" s="3" t="s">
-        <v>304</v>
+        <v>254</v>
+      </c>
+      <c r="B156" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>302</v>
-      </c>
-      <c r="B157" s="3" t="s">
-        <v>309</v>
+        <v>256</v>
+      </c>
+      <c r="B157" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>311</v>
-      </c>
-      <c r="B158" s="3" t="s">
-        <v>313</v>
+        <v>257</v>
+      </c>
+      <c r="B158" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>314</v>
-      </c>
-      <c r="B159" s="3" t="s">
-        <v>315</v>
+        <v>260</v>
+      </c>
+      <c r="B159" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
+        <v>270</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>271</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>272</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>273</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>278</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>280</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>289</v>
+      </c>
+      <c r="B166" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>291</v>
+      </c>
+      <c r="B167" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>293</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>295</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>296</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>297</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>306</v>
+      </c>
+      <c r="B172" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="B160" s="3" t="s">
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>308</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>310</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>315</v>
+      </c>
+      <c r="B175" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
         <v>321</v>
+      </c>
+      <c r="B176" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>322</v>
+      </c>
+      <c r="B177" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>323</v>
+      </c>
+      <c r="B178" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>324</v>
+      </c>
+      <c r="B179" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>330</v>
+      </c>
+      <c r="B180" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>333</v>
+      </c>
+      <c r="B181" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>336</v>
+      </c>
+      <c r="B182" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>337</v>
+      </c>
+      <c r="B183" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>347</v>
+      </c>
+      <c r="B184" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>349</v>
+      </c>
+      <c r="B185" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>352</v>
+      </c>
+      <c r="B186" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>381</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>383</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>385</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>365</v>
+      </c>
+      <c r="B190" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>366</v>
+      </c>
+      <c r="B191" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>367</v>
+      </c>
+      <c r="B192" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>368</v>
+      </c>
+      <c r="B193" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>369</v>
+      </c>
+      <c r="B194" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>370</v>
+      </c>
+      <c r="B195" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>371</v>
+      </c>
+      <c r="B196" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>372</v>
+      </c>
+      <c r="B197" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated texts based on review.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E949AC62-CF2D-49F2-81D8-DC19257D0D02}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37984AB1-7D9F-45DD-87A5-EA2E3EC2E1CC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="3615" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31770" yWindow="2745" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -904,9 +904,6 @@
     <t>volatile_acquisition_dialog_4</t>
   </si>
   <si>
-    <t>These are data that are lost once the computer is shut down.</t>
-  </si>
-  <si>
     <t>The following are the kind of volatile data you will want to gather: system time, RAM, process information, network log, logged-on users' information, and cached data (command history, clipboard, print spool files).</t>
   </si>
   <si>
@@ -964,9 +961,6 @@
     <t>The labelling of items can depend on the department, and typically has a sequential number. In this case it is: the investigator’s initials, date, sequence number, sub-sequence number if attached from another item.</t>
   </si>
   <si>
-    <t>The Chain of Custody helps ensure that all the evidences gathered are genuine, and can be used at the court of law.</t>
-  </si>
-  <si>
     <t>chain_of_custody_dialog_2</t>
   </si>
   <si>
@@ -1000,9 +994,6 @@
     <t>Now that you are back in the lab, the first thing to do is grab the devices we need to investigate.</t>
   </si>
   <si>
-    <t>When doing digital forensics, it is best to avoid using the evidences directly when investigating. In this case, we will simply clone the disk drives.</t>
-  </si>
-  <si>
     <t>lab_intro_clone_dialog_1</t>
   </si>
   <si>
@@ -1198,13 +1189,22 @@
     <t>Notice the message above indicating your arrival.</t>
   </si>
   <si>
-    <t>As an investigator, it is important to log every steps during the investigation.</t>
-  </si>
-  <si>
     <t>These logs are needed for reviewing and evaluating the case.</t>
   </si>
   <si>
     <t>You can review the activity log at the bottom of the screen.</t>
+  </si>
+  <si>
+    <t>When doing digital forensics, it is best to avoid using the evidence directly when investigating. In this case, we will simply clone the disk drives.</t>
+  </si>
+  <si>
+    <t>The Chain of Custody helps ensure that all the evidence gathered is genuine, and can be used at the court of law.</t>
+  </si>
+  <si>
+    <t>This is data that is lost once the computer is shut down.</t>
+  </si>
+  <si>
+    <t>As an investigator, it is important to log every step during the investigation.</t>
   </si>
 </sst>
 </file>
@@ -1545,8 +1545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="B170" sqref="B170"/>
+    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="B161" sqref="B161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1691,10 +1691,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B16" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1731,10 +1731,10 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B21" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2102,7 +2102,7 @@
         <v>99</v>
       </c>
       <c r="B67" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -2110,7 +2110,7 @@
         <v>100</v>
       </c>
       <c r="B68" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -2118,7 +2118,7 @@
         <v>101</v>
       </c>
       <c r="B69" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2126,7 +2126,7 @@
         <v>102</v>
       </c>
       <c r="B70" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -2158,7 +2158,7 @@
         <v>252</v>
       </c>
       <c r="B74" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -2403,10 +2403,10 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B105" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -2510,55 +2510,55 @@
         <v>284</v>
       </c>
       <c r="B118" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B119" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
+        <v>306</v>
+      </c>
+      <c r="B120" t="s">
         <v>307</v>
-      </c>
-      <c r="B120" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B121" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B122" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B123" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B124" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -2603,18 +2603,18 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B130" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B131" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -2718,7 +2718,7 @@
         <v>248</v>
       </c>
       <c r="B144" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -2763,50 +2763,50 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
+        <v>295</v>
+      </c>
+      <c r="B150" s="3" t="s">
         <v>296</v>
-      </c>
-      <c r="B150" s="3" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B151" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B152" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B155" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -2846,7 +2846,7 @@
         <v>269</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -2854,7 +2854,7 @@
         <v>270</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -2862,7 +2862,7 @@
         <v>271</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -2870,7 +2870,7 @@
         <v>272</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -2902,7 +2902,7 @@
         <v>287</v>
       </c>
       <c r="B167" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -2918,7 +2918,7 @@
         <v>291</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>294</v>
+        <v>393</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -2926,7 +2926,7 @@
         <v>292</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -2934,215 +2934,215 @@
         <v>293</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
+        <v>301</v>
+      </c>
+      <c r="B173" s="3" t="s">
         <v>302</v>
-      </c>
-      <c r="B173" s="3" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
+        <v>303</v>
+      </c>
+      <c r="B174" s="3" t="s">
         <v>304</v>
-      </c>
-      <c r="B174" s="3" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B175" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B176" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B177" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B178" t="s">
-        <v>314</v>
+        <v>392</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B179" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B180" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B181" t="s">
-        <v>326</v>
+        <v>391</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B182" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B183" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B184" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B185" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B186" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B190" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B191" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B192" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B193" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B194" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B195" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B196" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B197" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>